<commit_message>
Malsha Nishadini - Added Report Generation
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/testdata.xlsx
+++ b/src/main/resources/testdata/testdata.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyDoc\TMSTestSuite\src\main\resources\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NewProjectTMS\TMSTestSuite\src\main\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC60426C-DA35-43AE-9247-4259A9603135}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE08C530-718F-43AB-87B6-FF6B4B68C8F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="1" xr2:uid="{8B78A8B0-54BF-4CC9-A151-9EF835125B8C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{8B78A8B0-54BF-4CC9-A151-9EF835125B8C}"/>
   </bookViews>
   <sheets>
     <sheet name="TourBooking" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -29,7 +29,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="73">
   <si>
     <t>TestCase</t>
   </si>
@@ -134,21 +133,9 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Verify that the user is able to successfully submit an enquiry by entering valid values for the all text fields</t>
-  </si>
-  <si>
-    <t>Malsha Nishadini</t>
-  </si>
-  <si>
-    <t>malsha@gmail.com</t>
-  </si>
-  <si>
     <t>Enquiry_01</t>
   </si>
   <si>
-    <t>Submit Enquiry</t>
-  </si>
-  <si>
     <t>TestCaseName</t>
   </si>
   <si>
@@ -243,13 +230,42 @@
   </si>
   <si>
     <t>Abiman</t>
+  </si>
+  <si>
+    <t>malshagmail.com</t>
+  </si>
+  <si>
+    <t>Verify that user is able to successfully submit an enquiry by entering valid values for all text fields</t>
+  </si>
+  <si>
+    <t>Validation Message</t>
+  </si>
+  <si>
+    <t>Success Message</t>
+  </si>
+  <si>
+    <t>SUCCESS:Enquiry Successfully submitted</t>
+  </si>
+  <si>
+    <t>Verify user is unable to submit an enquiry when enter invalid value for the Email text field</t>
+  </si>
+  <si>
+    <t>Test User</t>
+  </si>
+  <si>
+    <t>testuser@gmail.com</t>
+  </si>
+  <si>
+    <t>8712345673</t>
+  </si>
+  <si>
+    <t>Submitting Enquiry</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="8">
     <font>
       <sz val="11"/>
@@ -410,7 +426,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -474,7 +490,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -799,12 +824,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.453125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="13.81640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="11.81640625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="13.81640625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="37.26953125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="10.81640625" collapsed="true"/>
+    <col min="1" max="1" width="17.453125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.81640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.81640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.81640625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="37.26953125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.81640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -953,24 +978,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75852AD6-BFFC-40C8-9432-3F59924423D1}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="45.453125" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="16.0" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="16.7265625" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="19.453125" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="15.453125" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="14.26953125" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="15.1796875" collapsed="false"/>
+    <col min="1" max="1" width="45.453125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.453125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="19.453125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.453125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.453125" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="21.26953125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="6" t="s">
         <v>24</v>
       </c>
@@ -989,43 +1014,62 @@
       <c r="F1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="29">
+      <c r="G1" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="29">
       <c r="A2" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="22">
-        <v>7704859788</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>33</v>
-      </c>
       <c r="F2" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-    </row>
-    <row r="4" spans="1:7">
+        <v>72</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="H2" s="9"/>
+    </row>
+    <row r="3" spans="1:8" s="24" customFormat="1" ht="29">
+      <c r="A3" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="9"/>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="11"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
@@ -1033,8 +1077,9 @@
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="H4" s="11"/>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
@@ -1042,8 +1087,9 @@
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="H5" s="11"/>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="11"/>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
@@ -1051,6 +1097,7 @@
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1064,181 +1111,181 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1E1DA55-EA0D-4A71-9A65-FD9AABC90914}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="52.453125" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="22.0" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="21.7265625" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="16.81640625" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="16.54296875" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="19.1796875" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="22.453125" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" width="16.1796875" collapsed="false"/>
+    <col min="1" max="1" width="52.453125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.7265625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.81640625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.54296875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.1796875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22.453125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16.1796875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" customHeight="1">
       <c r="A1" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="F1" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="G1" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="H1" s="14" t="s">
         <v>38</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>42</v>
       </c>
       <c r="I1" s="15"/>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1">
       <c r="A2" s="16" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E2" s="17">
         <v>1000</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="I2" s="15"/>
     </row>
     <row r="3" spans="1:9" ht="12.75" customHeight="1">
       <c r="A3" s="16" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="H3" s="17" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="I3" s="15"/>
     </row>
     <row r="4" spans="1:9" ht="13.5" customHeight="1">
       <c r="A4" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4" s="17" t="s">
+      <c r="G4" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="H4" s="17" t="s">
         <v>45</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="G4" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="H4" s="17" t="s">
-        <v>49</v>
       </c>
       <c r="I4" s="15"/>
     </row>
     <row r="5" spans="1:9" ht="12.75" customHeight="1">
       <c r="A5" s="16" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E5" s="17">
         <v>300</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="I5" s="15"/>
     </row>
     <row r="6" spans="1:9" ht="18" customHeight="1">
       <c r="A6" s="16" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E6" s="17">
         <v>3000</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H6" s="17" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="I6" s="15"/>
     </row>
@@ -1279,29 +1326,29 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="18.7265625" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="16.26953125" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="22.26953125" collapsed="false"/>
+    <col min="1" max="1" width="18.7265625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.26953125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.26953125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17.25" customHeight="1">
       <c r="A1" s="18" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D1" s="15"/>
     </row>
     <row r="2" spans="1:4" ht="13.5" customHeight="1">
       <c r="A2" s="20" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C2" s="21">
         <v>771237895</v>
@@ -1320,6 +1367,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007E9E972F8FE0754E8E087E010E821A75" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8e57a340751a7b025842778dd5a11b0f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ddf9af15-bd69-426d-975d-e6c68d677c2e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fa77d5786faeb27f87283b2c1d541258" ns2:_="">
     <xsd:import namespace="ddf9af15-bd69-426d-975d-e6c68d677c2e"/>
@@ -1465,7 +1518,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1474,13 +1527,16 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CCBB512E-A748-4110-9A11-8A273865AE2F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E59D7CEA-2CAA-4AC6-9B58-BE8754AC6ABA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1498,19 +1554,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C95ABD1E-50DC-4D2E-9CE6-80DE24832C95}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CCBB512E-A748-4110-9A11-8A273865AE2F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Insertion of screenshot and adding db verification for the signup
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/testdata.xlsx
+++ b/src/main/resources/testdata/testdata.xlsx
@@ -5,18 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NewProjectTMS\TMSTestSuite\src\main\resources\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chinthana_senanayake\Desktop\Mini Project\Selenium\Latest Update\src\main\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE08C530-718F-43AB-87B6-FF6B4B68C8F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{504EE7FA-3677-40A7-9AE3-3FB47238CA49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{8B78A8B0-54BF-4CC9-A151-9EF835125B8C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{8B78A8B0-54BF-4CC9-A151-9EF835125B8C}"/>
   </bookViews>
   <sheets>
     <sheet name="TourBooking" sheetId="1" r:id="rId1"/>
     <sheet name="Enquiry" sheetId="2" r:id="rId2"/>
-    <sheet name="Package" sheetId="3" r:id="rId3"/>
-    <sheet name="UserProfile" sheetId="4" r:id="rId4"/>
+    <sheet name="Login-Admin" sheetId="5" r:id="rId3"/>
+    <sheet name="Login" sheetId="6" r:id="rId4"/>
+    <sheet name="Package" sheetId="3" r:id="rId5"/>
+    <sheet name="UserProfile" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="88">
   <si>
     <t>TestCase</t>
   </si>
@@ -261,12 +263,57 @@
   <si>
     <t>Submitting Enquiry</t>
   </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Test@123</t>
+  </si>
+  <si>
+    <t>msd</t>
+  </si>
+  <si>
+    <t>tehan@gmail.com</t>
+  </si>
+  <si>
+    <t>Login_01</t>
+  </si>
+  <si>
+    <t>Login_02</t>
+  </si>
+  <si>
+    <t>Login_03</t>
+  </si>
+  <si>
+    <t>Login_04</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>RepeatPassword</t>
+  </si>
+  <si>
+    <t>Ranuka</t>
+  </si>
+  <si>
+    <t>ranuka@gmail.comPassword@123</t>
+  </si>
+  <si>
+    <t>Password@123</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>anju@gmail.com</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -323,6 +370,18 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -426,7 +485,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -500,6 +559,18 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -980,8 +1051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75852AD6-BFFC-40C8-9432-3F59924423D1}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection sqref="A1:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1108,6 +1179,272 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5CD590F-E130-44B2-985D-30F1082BB585}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="48.1796875" customWidth="1"/>
+    <col min="2" max="2" width="18.7265625" customWidth="1"/>
+    <col min="3" max="3" width="24.26953125" customWidth="1"/>
+    <col min="4" max="4" width="17.453125" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="26.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="12"/>
+      <c r="B2" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" s="9"/>
+      <c r="F2" s="12"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="22"/>
+      <c r="B3" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="22"/>
+      <c r="B4" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="22"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{2C82C213-79BB-43BE-9E49-B8723727A7CC}"/>
+    <hyperlink ref="B2" r:id="rId2" display="anuj@gmail.com" xr:uid="{6F296ABC-0E5C-4EC0-9A92-C64A4BA10CDF}"/>
+    <hyperlink ref="B3" r:id="rId3" display="anuj@gmail.com" xr:uid="{12E5A6C7-1CBA-4597-860D-CDC562AC9B34}"/>
+    <hyperlink ref="B4" r:id="rId4" xr:uid="{F5858856-FE13-4B1D-BC79-636531690A17}"/>
+    <hyperlink ref="C4" r:id="rId5" xr:uid="{B76639D7-2D71-4454-AB9D-1AE790F5360E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3DFE16C-ED1A-43D8-BFB5-41C5D83A9805}">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="31" customWidth="1"/>
+    <col min="2" max="2" width="20.26953125" customWidth="1"/>
+    <col min="3" max="3" width="21.453125" customWidth="1"/>
+    <col min="4" max="4" width="16.6328125" customWidth="1"/>
+    <col min="5" max="5" width="13.7265625" customWidth="1"/>
+    <col min="6" max="6" width="17.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="29">
+      <c r="A1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="12"/>
+      <c r="B2" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" s="9"/>
+      <c r="F2" s="12"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="22"/>
+      <c r="B3" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="22"/>
+      <c r="B4" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="22"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="27"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="12"/>
+      <c r="B9" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="10">
+        <v>776778985</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="E9" s="9"/>
+      <c r="F9" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{762F2F1B-873B-49B1-B140-22518DEADC81}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{8B269A1C-40F1-41F7-9D83-91FAA4410DA9}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{584DA329-5BE5-4C28-A74C-0424A842A650}"/>
+    <hyperlink ref="B4" r:id="rId4" xr:uid="{3E2FE625-04DC-4385-85D0-69A8EAC6AF34}"/>
+    <hyperlink ref="C4" r:id="rId5" xr:uid="{CEB25A16-F4BE-4666-9FE0-39AFB65BB392}"/>
+    <hyperlink ref="C9" r:id="rId6" display="Test@123" xr:uid="{3076FE8C-08C9-4319-820A-C627C6A478B1}"/>
+    <hyperlink ref="B9" r:id="rId7" display="anuj@gmail.com" xr:uid="{324CD73C-290D-40D5-846B-C7106DA55470}"/>
+    <hyperlink ref="D9" r:id="rId8" xr:uid="{D16BDD1A-8CE5-4262-A796-71962AD49AF1}"/>
+    <hyperlink ref="F9" r:id="rId9" xr:uid="{6F3950E6-E21F-4666-B363-FBDA69BC1693}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1E1DA55-EA0D-4A71-9A65-FD9AABC90914}">
   <dimension ref="A1:I8"/>
   <sheetViews>
@@ -1316,7 +1653,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4B37F18-6277-46FA-87B4-BA333166A713}">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -1367,12 +1704,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007E9E972F8FE0754E8E087E010E821A75" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8e57a340751a7b025842778dd5a11b0f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ddf9af15-bd69-426d-975d-e6c68d677c2e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fa77d5786faeb27f87283b2c1d541258" ns2:_="">
     <xsd:import namespace="ddf9af15-bd69-426d-975d-e6c68d677c2e"/>
@@ -1518,6 +1849,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1528,15 +1865,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CCBB512E-A748-4110-9A11-8A273865AE2F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E59D7CEA-2CAA-4AC6-9B58-BE8754AC6ABA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1554,6 +1882,15 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CCBB512E-A748-4110-9A11-8A273865AE2F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C95ABD1E-50DC-4D2E-9CE6-80DE24832C95}">
   <ds:schemaRefs>

</xml_diff>